<commit_message>
Task 3.5 (Fixes in Excel spreadsheets & plotting dynamics of sports achievements by gold medals)
</commit_message>
<xml_diff>
--- a/olympiad_analysis/gold_medals.xlsx
+++ b/olympiad_analysis/gold_medals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rexandel\Desktop\GitHub\big_data_research\olympiad_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97566DF-A8E2-4F85-9836-A7D74CC1720C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A9484B-EF19-4E54-BB96-C2419B6919B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,12 +211,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -224,6 +218,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -507,7 +507,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,185 +526,186 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5">
-        <v>11</v>
-      </c>
-      <c r="D2" s="5">
         <v>6</v>
       </c>
-      <c r="E2" s="5">
-        <v>4</v>
-      </c>
-      <c r="F2" s="5">
-        <v>8</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="B2" s="3">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3">
         <v>6</v>
       </c>
-      <c r="H2" s="6">
-        <v>7</v>
+      <c r="F2" s="3">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3</v>
+      </c>
+      <c r="H2" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="C3" s="3">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3">
         <v>9</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
         <v>9</v>
       </c>
-      <c r="F3" s="5">
-        <v>8</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="H3" s="4">
         <v>5</v>
-      </c>
-      <c r="H3" s="6">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3">
         <v>10</v>
       </c>
-      <c r="C4" s="5">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5">
-        <v>10</v>
-      </c>
-      <c r="F4" s="5">
-        <v>5</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="D4" s="3">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3">
         <v>4</v>
       </c>
-      <c r="H4" s="6">
+      <c r="G4" s="3">
+        <v>4</v>
+      </c>
+      <c r="H4" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5">
-        <v>9</v>
-      </c>
-      <c r="E5" s="5">
-        <v>13</v>
-      </c>
-      <c r="F5" s="5">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5">
-        <v>4</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="5">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5">
-        <v>7</v>
-      </c>
-      <c r="F6" s="5">
-        <v>3</v>
-      </c>
-      <c r="G6" s="5">
-        <v>9</v>
-      </c>
-      <c r="H6" s="6">
-        <v>5</v>
+      <c r="H6" s="4">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="6">
+        <v>15</v>
+      </c>
+      <c r="C7" s="6">
+        <v>11</v>
+      </c>
+      <c r="D7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="8">
-        <v>13</v>
-      </c>
-      <c r="C7" s="8">
-        <v>12</v>
-      </c>
-      <c r="D7" s="8">
-        <v>10</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
+        <v>4</v>
+      </c>
+      <c r="F7" s="6">
+        <v>8</v>
+      </c>
+      <c r="G7" s="6">
         <v>6</v>
       </c>
-      <c r="F7" s="8">
-        <v>3</v>
-      </c>
-      <c r="G7" s="8">
-        <v>3</v>
-      </c>
-      <c r="H7" s="9">
-        <v>3</v>
+      <c r="H7" s="7">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>